<commit_message>
modif createSortedListWithNValues(int n) + fractionned code + add Iterative Delete
</commit_message>
<xml_diff>
--- a/classeur PRJT C.xlsx
+++ b/classeur PRJT C.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45e349c677ad452e/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Directory C\PROJET-C-L2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03D1617B-7DD8-4450-9A2E-6FAEC394FE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81C291-09DF-42D3-AD76-1417A8DC9B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7BBA2EEE-4B54-4C74-A655-83493E93B4F0}"/>
   </bookViews>
@@ -36,11 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -79,11 +75,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,72 +165,84 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$B$21</c:f>
+              <c:f>Feuil1!$B$1:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>125</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>279</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>666</c:v>
+                  <c:v>297</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1314</c:v>
+                  <c:v>598</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2657</c:v>
+                  <c:v>1375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5713</c:v>
+                  <c:v>3292</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20631</c:v>
+                  <c:v>10367</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75273</c:v>
+                  <c:v>31827</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>169804</c:v>
+                  <c:v>86799</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>343700</c:v>
+                  <c:v>168442</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>352269</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>741422</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1364749</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2715439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -241,7 +250,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1733-4620-A9D9-BECB3ED61ACF}"/>
+              <c16:uniqueId val="{00000000-90C0-4B63-95F8-30B79CD443BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -254,11 +263,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1976157087"/>
-        <c:axId val="36200559"/>
+        <c:axId val="931429792"/>
+        <c:axId val="1027787616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1976157087"/>
+        <c:axId val="931429792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +309,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36200559"/>
+        <c:crossAx val="1027787616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -308,7 +317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36200559"/>
+        <c:axId val="1027787616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +368,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1976157087"/>
+        <c:crossAx val="931429792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -482,72 +491,87 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$J$1:$J$21</c:f>
+              <c:f>Feuil1!$J$1:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,7 +579,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9953-4D19-ADCB-3E344CB40F90}"/>
+              <c16:uniqueId val="{00000000-CE8C-494B-B2C6-AFA10F8807ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -568,11 +592,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="30913695"/>
-        <c:axId val="1981081119"/>
+        <c:axId val="934398480"/>
+        <c:axId val="1223880304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30913695"/>
+        <c:axId val="934398480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +638,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1981081119"/>
+        <c:crossAx val="1223880304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -622,10 +646,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1981081119"/>
+        <c:axId val="1223880304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="400000"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -674,7 +698,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30913695"/>
+        <c:crossAx val="934398480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1847,22 +1871,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
+      <xdr:colOff>624840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3">
+        <xdr:cNvPr id="3" name="Graphique 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F56FDC7D-D852-14FB-2028-442CA6D027D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5921D91-E41F-97F0-02C7-D25588749A23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,23 +1906,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4">
+        <xdr:cNvPr id="6" name="Graphique 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A756EC00-FB4A-4D36-34B5-BECCBC977E08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AAAD0B2-5FCA-5354-BEEB-01A4B71A78C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2216,13 +2240,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC09835A-5000-421F-900D-E64EBF0AD2C7}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="2"/>
+    <col min="9" max="9" width="11.5546875" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1">
@@ -2235,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="J1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2243,13 +2271,13 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2257,13 +2285,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2271,13 +2299,13 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2285,10 +2313,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2299,13 +2327,13 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2313,13 +2341,13 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2327,13 +2355,13 @@
         <v>8</v>
       </c>
       <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
         <v>7</v>
       </c>
-      <c r="I8" s="1">
-        <v>8</v>
-      </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2341,13 +2369,13 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2355,13 +2383,13 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2369,13 +2397,13 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="I11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2383,13 +2411,13 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2397,10 +2425,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>279</v>
+        <v>137</v>
       </c>
       <c r="I13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2411,13 +2439,13 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>666</v>
+        <v>297</v>
       </c>
       <c r="I14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2425,13 +2453,13 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>1314</v>
+        <v>598</v>
       </c>
       <c r="I15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2439,13 +2467,13 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>2657</v>
+        <v>1375</v>
       </c>
       <c r="I16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2453,13 +2481,13 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>5713</v>
+        <v>3292</v>
       </c>
       <c r="I17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2467,13 +2495,13 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>20631</v>
+        <v>10367</v>
       </c>
       <c r="I18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2481,13 +2509,13 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>75273</v>
+        <v>31827</v>
       </c>
       <c r="I19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2495,13 +2523,13 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>169804</v>
+        <v>86799</v>
       </c>
       <c r="I20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2509,16 +2537,77 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>343700</v>
-      </c>
-      <c r="E21" t="s">
-        <v>0</v>
+        <v>168442</v>
       </c>
       <c r="I21" s="1">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>352269</v>
+      </c>
+      <c r="I22" s="1">
         <v>21</v>
       </c>
-      <c r="J21">
-        <v>1</v>
+      <c r="J22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>741422</v>
+      </c>
+      <c r="I23" s="1">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1364749</v>
+      </c>
+      <c r="I24" s="1">
+        <v>23</v>
+      </c>
+      <c r="J24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2715439</v>
+      </c>
+      <c r="I25" s="1">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="I26" s="1">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>